<commit_message>
bug fix & list machine with ecart
</commit_message>
<xml_diff>
--- a/verification.xlsx
+++ b/verification.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryrab\Desktop\Ryan\Etudes\S5\ArchitectureLogiciel\Matelas\matelas\Matelas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CEDFB2-AD1F-4B7D-8398-6FC91A00431F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D6D90A-B8A7-442A-9022-78174CD7E11D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F949108E-545E-468F-AB23-EB4DEEB7D26F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{F949108E-545E-468F-AB23-EB4DEEB7D26F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="47">
   <si>
     <t>nom block</t>
   </si>
@@ -97,13 +98,92 @@
   </si>
   <si>
     <t>restes</t>
+  </si>
+  <si>
+    <t>Matelas 1</t>
+  </si>
+  <si>
+    <t>Matelas 2</t>
+  </si>
+  <si>
+    <t>Matelas 3</t>
+  </si>
+  <si>
+    <t>Matelas 4</t>
+  </si>
+  <si>
+    <t>Matelas 5</t>
+  </si>
+  <si>
+    <t>Matelas 6</t>
+  </si>
+  <si>
+    <t>Matelas 7</t>
+  </si>
+  <si>
+    <t>Matelas 8</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Matelas</t>
+  </si>
+  <si>
+    <t>Longueur</t>
+  </si>
+  <si>
+    <t>Largueur</t>
+  </si>
+  <si>
+    <t>Epaisseur</t>
+  </si>
+  <si>
+    <t>Prix unitaire</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Matiere premiere</t>
+  </si>
+  <si>
+    <t>Essence</t>
+  </si>
+  <si>
+    <t>Qte</t>
+  </si>
+  <si>
+    <t>Papier</t>
+  </si>
+  <si>
+    <t>Durcisseur</t>
+  </si>
+  <si>
+    <t>QteVoulu</t>
+  </si>
+  <si>
+    <t>IdMatierePremiere</t>
+  </si>
+  <si>
+    <t>Somme</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,7 +212,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -140,17 +220,75 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Milliers" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -465,7 +603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04B8FD34-947E-4DD0-9FCB-59D241BD3586}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -804,4 +942,758 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DFD3DB8-1C1A-4217-96AF-35D3790EC1EF}">
+  <dimension ref="A1:P27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="6">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6">
+        <v>23.21</v>
+      </c>
+      <c r="E2" s="6">
+        <v>13.12</v>
+      </c>
+      <c r="F2" s="6">
+        <v>1000000</v>
+      </c>
+      <c r="G2" s="5">
+        <f>C2*D2*E2</f>
+        <v>913.54559999999992</v>
+      </c>
+      <c r="I2" s="4">
+        <v>1</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="D3" s="6">
+        <v>24.44</v>
+      </c>
+      <c r="E3" s="6">
+        <v>12.99</v>
+      </c>
+      <c r="F3" s="6">
+        <v>2500000</v>
+      </c>
+      <c r="G3" s="5">
+        <f t="shared" ref="G3:G11" si="0">C3*D3*E3</f>
+        <v>692.09680800000012</v>
+      </c>
+      <c r="I3" s="4">
+        <v>2</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="6">
+        <v>5.59</v>
+      </c>
+      <c r="D4" s="6">
+        <v>23.36</v>
+      </c>
+      <c r="E4" s="6">
+        <v>10.38</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1781361.34</v>
+      </c>
+      <c r="G4" s="5">
+        <f t="shared" si="0"/>
+        <v>1355.4453120000003</v>
+      </c>
+      <c r="I4" s="4">
+        <v>3</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="6">
+        <v>6.98</v>
+      </c>
+      <c r="D5" s="6">
+        <v>23.03</v>
+      </c>
+      <c r="E5" s="6">
+        <v>10.220000000000001</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1621366.8</v>
+      </c>
+      <c r="G5" s="5">
+        <f t="shared" si="0"/>
+        <v>1642.8588680000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="6">
+        <v>6.57</v>
+      </c>
+      <c r="D6" s="6">
+        <v>23.22</v>
+      </c>
+      <c r="E6" s="6">
+        <v>10.8</v>
+      </c>
+      <c r="F6" s="6">
+        <v>1780942.76</v>
+      </c>
+      <c r="G6" s="5">
+        <f t="shared" si="0"/>
+        <v>1647.5983200000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="6">
+        <v>6.63</v>
+      </c>
+      <c r="D7" s="6">
+        <v>20.54</v>
+      </c>
+      <c r="E7" s="6">
+        <v>10.53</v>
+      </c>
+      <c r="F7" s="6">
+        <v>1722190.6</v>
+      </c>
+      <c r="G7" s="5">
+        <f t="shared" si="0"/>
+        <v>1433.9775059999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="6">
+        <v>5.7</v>
+      </c>
+      <c r="D8" s="6">
+        <v>23.61</v>
+      </c>
+      <c r="E8" s="6">
+        <v>13.19</v>
+      </c>
+      <c r="F8" s="6">
+        <v>1842178.89</v>
+      </c>
+      <c r="G8" s="5">
+        <f t="shared" si="0"/>
+        <v>1775.0706299999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="6">
+        <v>6.35</v>
+      </c>
+      <c r="D9" s="6">
+        <v>20.62</v>
+      </c>
+      <c r="E9" s="6">
+        <v>13.14</v>
+      </c>
+      <c r="F9" s="6">
+        <v>1919412.89</v>
+      </c>
+      <c r="G9" s="5">
+        <f t="shared" si="0"/>
+        <v>1720.5121800000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="6">
+        <v>5.59</v>
+      </c>
+      <c r="D10" s="6">
+        <v>22.85</v>
+      </c>
+      <c r="E10" s="6">
+        <v>12.56</v>
+      </c>
+      <c r="F10" s="6">
+        <v>1899911.84</v>
+      </c>
+      <c r="G10" s="5">
+        <f t="shared" si="0"/>
+        <v>1604.3076400000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="6">
+        <v>6</v>
+      </c>
+      <c r="D11" s="6">
+        <v>21.75</v>
+      </c>
+      <c r="E11" s="6">
+        <v>10.09</v>
+      </c>
+      <c r="F11" s="6">
+        <v>1676884.75</v>
+      </c>
+      <c r="G11" s="5">
+        <f t="shared" si="0"/>
+        <v>1316.7449999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="D14" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="G14" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" s="10"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="P15" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
+        <v>1</v>
+      </c>
+      <c r="B16" s="6">
+        <f>G2*$K$2</f>
+        <v>1827.0911999999998</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
+      <c r="E16" s="6">
+        <f>G2*$K$3</f>
+        <v>2740.6367999999998</v>
+      </c>
+      <c r="G16" s="4">
+        <v>1</v>
+      </c>
+      <c r="H16" s="6">
+        <f>G2*$K$4</f>
+        <v>456.77279999999996</v>
+      </c>
+      <c r="J16" s="4">
+        <v>1</v>
+      </c>
+      <c r="K16" s="4">
+        <v>5750</v>
+      </c>
+      <c r="L16" s="4">
+        <v>750</v>
+      </c>
+      <c r="N16" s="4">
+        <v>2</v>
+      </c>
+      <c r="O16" s="4">
+        <v>10750</v>
+      </c>
+      <c r="P16" s="4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <v>2</v>
+      </c>
+      <c r="B17" s="6">
+        <f>G3*$K$2</f>
+        <v>1384.1936160000002</v>
+      </c>
+      <c r="D17" s="4">
+        <v>2</v>
+      </c>
+      <c r="E17" s="6">
+        <f>G3*$K$3</f>
+        <v>2076.2904240000003</v>
+      </c>
+      <c r="G17" s="4">
+        <v>2</v>
+      </c>
+      <c r="H17" s="6">
+        <f>G3*$K$4</f>
+        <v>346.04840400000006</v>
+      </c>
+      <c r="J17" s="4">
+        <v>1</v>
+      </c>
+      <c r="K17" s="4">
+        <v>5325</v>
+      </c>
+      <c r="L17" s="4">
+        <v>825</v>
+      </c>
+      <c r="N17" s="4">
+        <v>2</v>
+      </c>
+      <c r="O17" s="4">
+        <v>12532</v>
+      </c>
+      <c r="P17" s="4">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>3</v>
+      </c>
+      <c r="B18" s="6">
+        <f>G4*$K$2</f>
+        <v>2710.8906240000006</v>
+      </c>
+      <c r="D18" s="4">
+        <v>3</v>
+      </c>
+      <c r="E18" s="6">
+        <f>G4*$K$3</f>
+        <v>4066.3359360000009</v>
+      </c>
+      <c r="G18" s="4">
+        <v>3</v>
+      </c>
+      <c r="H18" s="6">
+        <f>G4*$K$4</f>
+        <v>677.72265600000014</v>
+      </c>
+      <c r="J18" s="4">
+        <v>1</v>
+      </c>
+      <c r="K18" s="4">
+        <v>6324</v>
+      </c>
+      <c r="L18" s="4">
+        <v>660</v>
+      </c>
+      <c r="N18" s="4">
+        <v>2</v>
+      </c>
+      <c r="O18" s="4">
+        <v>23546</v>
+      </c>
+      <c r="P18" s="4">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <v>4</v>
+      </c>
+      <c r="B19" s="6">
+        <f>G5*$K$2</f>
+        <v>3285.7177360000005</v>
+      </c>
+      <c r="D19" s="4">
+        <v>4</v>
+      </c>
+      <c r="E19" s="6">
+        <f>G5*$K$3</f>
+        <v>4928.5766040000008</v>
+      </c>
+      <c r="G19" s="4">
+        <v>4</v>
+      </c>
+      <c r="H19" s="6">
+        <f>G5*$K$4</f>
+        <v>821.42943400000013</v>
+      </c>
+      <c r="J19" s="4">
+        <v>1</v>
+      </c>
+      <c r="K19" s="4">
+        <v>5235</v>
+      </c>
+      <c r="L19" s="4">
+        <v>720</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="O19" s="4">
+        <f>SUM(O16:O18)</f>
+        <v>46828</v>
+      </c>
+      <c r="P19" s="12"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>5</v>
+      </c>
+      <c r="B20" s="6">
+        <f>G6*$K$2</f>
+        <v>3295.1966400000001</v>
+      </c>
+      <c r="D20" s="4">
+        <v>5</v>
+      </c>
+      <c r="E20" s="6">
+        <f>G6*$K$3</f>
+        <v>4942.7949600000002</v>
+      </c>
+      <c r="G20" s="4">
+        <v>5</v>
+      </c>
+      <c r="H20" s="6">
+        <f>G6*$K$4</f>
+        <v>823.79916000000003</v>
+      </c>
+      <c r="J20" s="4">
+        <v>1</v>
+      </c>
+      <c r="K20" s="4">
+        <v>6532</v>
+      </c>
+      <c r="L20" s="4">
+        <v>925</v>
+      </c>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>6</v>
+      </c>
+      <c r="B21" s="6">
+        <f>G7*$K$2</f>
+        <v>2867.9550119999994</v>
+      </c>
+      <c r="D21" s="4">
+        <v>6</v>
+      </c>
+      <c r="E21" s="6">
+        <f>G7*$K$3</f>
+        <v>4301.9325179999996</v>
+      </c>
+      <c r="G21" s="4">
+        <v>6</v>
+      </c>
+      <c r="H21" s="6">
+        <f>G7*$K$4</f>
+        <v>716.98875299999986</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K21" s="4">
+        <f>SUM(K16:K20)</f>
+        <v>29166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <v>7</v>
+      </c>
+      <c r="B22" s="6">
+        <f>G8*$K$2</f>
+        <v>3550.1412599999999</v>
+      </c>
+      <c r="D22" s="4">
+        <v>7</v>
+      </c>
+      <c r="E22" s="6">
+        <f>G8*$K$3</f>
+        <v>5325.2118899999996</v>
+      </c>
+      <c r="G22" s="4">
+        <v>7</v>
+      </c>
+      <c r="H22" s="6">
+        <f>G8*$K$4</f>
+        <v>887.53531499999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" s="4">
+        <v>8</v>
+      </c>
+      <c r="B23" s="6">
+        <f>G9*$K$2</f>
+        <v>3441.0243600000003</v>
+      </c>
+      <c r="D23" s="4">
+        <v>8</v>
+      </c>
+      <c r="E23" s="6">
+        <f>G9*$K$3</f>
+        <v>5161.536540000001</v>
+      </c>
+      <c r="G23" s="4">
+        <v>8</v>
+      </c>
+      <c r="H23" s="6">
+        <f>G9*$K$4</f>
+        <v>860.25609000000009</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
+        <v>9</v>
+      </c>
+      <c r="B24" s="6">
+        <f>G10*$K$2</f>
+        <v>3208.6152800000004</v>
+      </c>
+      <c r="D24" s="4">
+        <v>9</v>
+      </c>
+      <c r="E24" s="6">
+        <f>G10*$K$3</f>
+        <v>4812.9229200000009</v>
+      </c>
+      <c r="G24" s="4">
+        <v>9</v>
+      </c>
+      <c r="H24" s="6">
+        <f>G10*$K$4</f>
+        <v>802.15382000000011</v>
+      </c>
+      <c r="J24" s="4">
+        <v>3</v>
+      </c>
+      <c r="K24" s="4">
+        <v>5750</v>
+      </c>
+      <c r="L24" s="4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" s="4">
+        <v>10</v>
+      </c>
+      <c r="B25" s="6">
+        <f>G11*$K$2</f>
+        <v>2633.49</v>
+      </c>
+      <c r="D25" s="4">
+        <v>10</v>
+      </c>
+      <c r="E25" s="6">
+        <f>G11*$K$3</f>
+        <v>3950.2349999999997</v>
+      </c>
+      <c r="G25" s="4">
+        <v>10</v>
+      </c>
+      <c r="H25" s="6">
+        <f>G11*$K$4</f>
+        <v>658.37249999999995</v>
+      </c>
+      <c r="J25" s="4">
+        <v>3</v>
+      </c>
+      <c r="K25" s="4">
+        <v>3532</v>
+      </c>
+      <c r="L25" s="4">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="11">
+        <f>SUM(B16:B25)</f>
+        <v>28204.315728000001</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="11">
+        <f>SUM(E16:E25)</f>
+        <v>42306.473591999995</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H26" s="11">
+        <f>SUM(H16:H25)</f>
+        <v>7051.0789320000003</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K26" s="4">
+        <f>SUM(K24:K25)</f>
+        <v>9282</v>
+      </c>
+      <c r="L26" s="12"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="L27" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
bug fix prix théorique
</commit_message>
<xml_diff>
--- a/verification.xlsx
+++ b/verification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryrab\Desktop\Ryan\Etudes\S5\ArchitectureLogiciel\Matelas\matelas\Matelas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D6D90A-B8A7-442A-9022-78174CD7E11D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC7ADE44-0FE5-4EF8-95A5-535953B29E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{F949108E-545E-468F-AB23-EB4DEEB7D26F}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="50">
   <si>
     <t>nom block</t>
   </si>
@@ -167,14 +167,25 @@
   </si>
   <si>
     <t>Somme</t>
+  </si>
+  <si>
+    <t>IdMatelas</t>
+  </si>
+  <si>
+    <t>Prix théorique</t>
+  </si>
+  <si>
+    <t>PT/V</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.000\ _€_-;\-* #,##0.000\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -274,7 +285,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -285,7 +295,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Milliers" xfId="1" builtinId="3"/>
@@ -946,21 +957,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DFD3DB8-1C1A-4217-96AF-35D3790EC1EF}">
-  <dimension ref="A1:P27"/>
+  <dimension ref="A1:V34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
@@ -979,7 +994,7 @@
       <c r="F1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="4" t="s">
         <v>38</v>
       </c>
       <c r="I1" s="4" t="s">
@@ -992,7 +1007,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1025,7 +1040,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1058,7 +1073,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1091,7 +1106,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1115,7 +1130,7 @@
         <v>1642.8588680000003</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1139,7 +1154,7 @@
         <v>1647.5983200000001</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1163,7 +1178,7 @@
         <v>1433.9775059999997</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1187,7 +1202,7 @@
         <v>1775.0706299999999</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1211,7 +1226,7 @@
         <v>1720.5121800000002</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1235,7 +1250,7 @@
         <v>1604.3076400000002</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1259,438 +1274,604 @@
         <v>1316.7449999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="D14" s="9" t="s">
+      <c r="B14" s="7"/>
+      <c r="F14" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="10"/>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="9"/>
+      <c r="K14" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="H14" s="10"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="G15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="K15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="L15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="P15" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="Q15" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L15" s="4" t="s">
+      <c r="R15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N15" s="4" t="s">
+      <c r="T15" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="O15" s="4" t="s">
+      <c r="U15" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="P15" s="4" t="s">
+      <c r="V15" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>1</v>
       </c>
       <c r="B16" s="6">
-        <f>G2*$K$2</f>
+        <f t="shared" ref="B16:B25" si="1">G2*$K$2</f>
         <v>1827.0911999999998</v>
       </c>
-      <c r="D16" s="4">
+      <c r="C16" s="11">
+        <f>B16*R16</f>
+        <v>1370318.4</v>
+      </c>
+      <c r="D16" s="11">
+        <f>Q16-B16</f>
+        <v>3922.9088000000002</v>
+      </c>
+      <c r="F16" s="4">
         <v>1</v>
       </c>
-      <c r="E16" s="6">
+      <c r="G16" s="6">
         <f>G2*$K$3</f>
         <v>2740.6367999999998</v>
       </c>
-      <c r="G16" s="4">
+      <c r="H16" s="11">
+        <f>G16*V16</f>
+        <v>1370318.4</v>
+      </c>
+      <c r="I16" s="11">
+        <f>U16-G16</f>
+        <v>8009.3631999999998</v>
+      </c>
+      <c r="K16" s="4">
         <v>1</v>
       </c>
-      <c r="H16" s="6">
+      <c r="L16" s="6">
         <f>G2*$K$4</f>
         <v>456.77279999999996</v>
       </c>
-      <c r="J16" s="4">
+      <c r="M16" s="11">
+        <f>L16*R24</f>
+        <v>228386.4</v>
+      </c>
+      <c r="N16" s="11">
+        <f>Q24-L16</f>
+        <v>5293.2272000000003</v>
+      </c>
+      <c r="P16" s="4">
         <v>1</v>
       </c>
-      <c r="K16" s="4">
+      <c r="Q16" s="4">
         <v>5750</v>
       </c>
-      <c r="L16" s="4">
+      <c r="R16" s="4">
         <v>750</v>
       </c>
-      <c r="N16" s="4">
+      <c r="T16" s="4">
         <v>2</v>
       </c>
-      <c r="O16" s="4">
+      <c r="U16" s="4">
         <v>10750</v>
       </c>
-      <c r="P16" s="4">
+      <c r="V16" s="4">
         <v>500</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>2</v>
       </c>
       <c r="B17" s="6">
-        <f>G3*$K$2</f>
+        <f t="shared" si="1"/>
         <v>1384.1936160000002</v>
       </c>
-      <c r="D17" s="4">
+      <c r="C17" s="11">
+        <f>R16*B17</f>
+        <v>1038145.2120000002</v>
+      </c>
+      <c r="D17" s="11">
+        <f>D16-B17</f>
+        <v>2538.7151839999997</v>
+      </c>
+      <c r="F17" s="4">
         <v>2</v>
       </c>
-      <c r="E17" s="6">
+      <c r="G17" s="6">
         <f>G3*$K$3</f>
         <v>2076.2904240000003</v>
       </c>
-      <c r="G17" s="4">
+      <c r="H17" s="11">
+        <f>G17*V16</f>
+        <v>1038145.2120000002</v>
+      </c>
+      <c r="I17" s="11">
+        <f>I16-G17</f>
+        <v>5933.0727759999991</v>
+      </c>
+      <c r="K17" s="4">
         <v>2</v>
       </c>
-      <c r="H17" s="6">
+      <c r="L17" s="6">
         <f>G3*$K$4</f>
         <v>346.04840400000006</v>
       </c>
-      <c r="J17" s="4">
+      <c r="M17" s="11">
+        <f>R24*L17</f>
+        <v>173024.20200000002</v>
+      </c>
+      <c r="N17" s="11">
+        <f>N16-L17</f>
+        <v>4947.1787960000001</v>
+      </c>
+      <c r="P17" s="4">
         <v>1</v>
       </c>
-      <c r="K17" s="4">
+      <c r="Q17" s="4">
         <v>5325</v>
       </c>
-      <c r="L17" s="4">
+      <c r="R17" s="4">
         <v>825</v>
       </c>
-      <c r="N17" s="4">
+      <c r="T17" s="4">
         <v>2</v>
       </c>
-      <c r="O17" s="4">
+      <c r="U17" s="4">
         <v>12532</v>
       </c>
-      <c r="P17" s="4">
+      <c r="V17" s="4">
         <v>750</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>3</v>
       </c>
       <c r="B18" s="6">
-        <f>G4*$K$2</f>
+        <f t="shared" si="1"/>
         <v>2710.8906240000006</v>
       </c>
-      <c r="D18" s="4">
+      <c r="C18" s="11">
+        <f>(D17*R16)+((B18-D17)*R17)</f>
+        <v>2046081.1260000006</v>
+      </c>
+      <c r="D18" s="11">
+        <f>Q17-(B18-D17)</f>
+        <v>5152.8245599999991</v>
+      </c>
+      <c r="E18" s="12">
+        <f>((B18-D17)*R17)</f>
+        <v>142044.73800000074</v>
+      </c>
+      <c r="F18" s="4">
         <v>3</v>
       </c>
-      <c r="E18" s="6">
+      <c r="G18" s="6">
         <f>G4*$K$3</f>
         <v>4066.3359360000009</v>
       </c>
-      <c r="G18" s="4">
+      <c r="H18" s="11">
+        <f>G18*V16</f>
+        <v>2033167.9680000003</v>
+      </c>
+      <c r="I18" s="11">
+        <f>I17-G18</f>
+        <v>1866.7368399999982</v>
+      </c>
+      <c r="K18" s="4">
         <v>3</v>
       </c>
-      <c r="H18" s="6">
+      <c r="L18" s="6">
         <f>G4*$K$4</f>
         <v>677.72265600000014</v>
       </c>
-      <c r="J18" s="4">
+      <c r="M18" s="11">
+        <f>R24*L18</f>
+        <v>338861.3280000001</v>
+      </c>
+      <c r="N18" s="11">
+        <f>N17-L18</f>
+        <v>4269.4561400000002</v>
+      </c>
+      <c r="P18" s="4">
         <v>1</v>
       </c>
-      <c r="K18" s="4">
+      <c r="Q18" s="4">
         <v>6324</v>
       </c>
-      <c r="L18" s="4">
+      <c r="R18" s="4">
         <v>660</v>
       </c>
-      <c r="N18" s="4">
+      <c r="T18" s="4">
         <v>2</v>
       </c>
-      <c r="O18" s="4">
+      <c r="U18" s="4">
         <v>23546</v>
       </c>
-      <c r="P18" s="4">
+      <c r="V18" s="4">
         <v>450</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>4</v>
       </c>
       <c r="B19" s="6">
-        <f>G5*$K$2</f>
+        <f t="shared" si="1"/>
         <v>3285.7177360000005</v>
       </c>
-      <c r="D19" s="4">
+      <c r="C19" s="11">
+        <f>B19*R17</f>
+        <v>2710717.1322000003</v>
+      </c>
+      <c r="F19" s="4">
         <v>4</v>
       </c>
-      <c r="E19" s="6">
+      <c r="G19" s="6">
         <f>G5*$K$3</f>
         <v>4928.5766040000008</v>
       </c>
-      <c r="G19" s="4">
+      <c r="H19" s="11">
+        <f>(I18*V16)+((G19-I18)*V17)</f>
+        <v>3229748.2430000007</v>
+      </c>
+      <c r="K19" s="4">
         <v>4</v>
       </c>
-      <c r="H19" s="6">
+      <c r="L19" s="6">
         <f>G5*$K$4</f>
         <v>821.42943400000013</v>
       </c>
-      <c r="J19" s="4">
+      <c r="M19" s="11">
+        <f>L19*R24</f>
+        <v>410714.71700000006</v>
+      </c>
+      <c r="P19" s="4">
         <v>1</v>
       </c>
-      <c r="K19" s="4">
+      <c r="Q19" s="4">
         <v>5235</v>
       </c>
-      <c r="L19" s="4">
+      <c r="R19" s="4">
         <v>720</v>
       </c>
-      <c r="N19" s="4" t="s">
+      <c r="T19" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="O19" s="4">
-        <f>SUM(O16:O18)</f>
+      <c r="U19" s="4">
+        <f>SUM(U16:U18)</f>
         <v>46828</v>
       </c>
-      <c r="P19" s="12"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>5</v>
       </c>
       <c r="B20" s="6">
-        <f>G6*$K$2</f>
+        <f t="shared" si="1"/>
         <v>3295.1966400000001</v>
       </c>
-      <c r="D20" s="4">
+      <c r="F20" s="4">
         <v>5</v>
       </c>
-      <c r="E20" s="6">
+      <c r="G20" s="6">
         <f>G6*$K$3</f>
         <v>4942.7949600000002</v>
       </c>
-      <c r="G20" s="4">
+      <c r="K20" s="4">
         <v>5</v>
       </c>
-      <c r="H20" s="6">
+      <c r="L20" s="6">
         <f>G6*$K$4</f>
         <v>823.79916000000003</v>
       </c>
-      <c r="J20" s="4">
+      <c r="P20" s="4">
         <v>1</v>
       </c>
-      <c r="K20" s="4">
+      <c r="Q20" s="4">
         <v>6532</v>
       </c>
-      <c r="L20" s="4">
+      <c r="R20" s="4">
         <v>925</v>
       </c>
-      <c r="N20" s="12"/>
-      <c r="O20" s="12"/>
-      <c r="P20" s="12"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>6</v>
       </c>
       <c r="B21" s="6">
-        <f>G7*$K$2</f>
+        <f t="shared" si="1"/>
         <v>2867.9550119999994</v>
       </c>
-      <c r="D21" s="4">
+      <c r="F21" s="4">
         <v>6</v>
       </c>
-      <c r="E21" s="6">
+      <c r="G21" s="6">
         <f>G7*$K$3</f>
         <v>4301.9325179999996</v>
       </c>
-      <c r="G21" s="4">
+      <c r="K21" s="4">
         <v>6</v>
       </c>
-      <c r="H21" s="6">
+      <c r="L21" s="6">
         <f>G7*$K$4</f>
         <v>716.98875299999986</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="P21" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="K21" s="4">
-        <f>SUM(K16:K20)</f>
+      <c r="Q21" s="4">
+        <f>SUM(Q16:Q20)</f>
         <v>29166</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>7</v>
       </c>
       <c r="B22" s="6">
-        <f>G8*$K$2</f>
+        <f t="shared" si="1"/>
         <v>3550.1412599999999</v>
       </c>
-      <c r="D22" s="4">
+      <c r="F22" s="4">
         <v>7</v>
       </c>
-      <c r="E22" s="6">
+      <c r="G22" s="6">
         <f>G8*$K$3</f>
         <v>5325.2118899999996</v>
       </c>
-      <c r="G22" s="4">
+      <c r="K22" s="4">
         <v>7</v>
       </c>
-      <c r="H22" s="6">
+      <c r="L22" s="6">
         <f>G8*$K$4</f>
         <v>887.53531499999997</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>8</v>
       </c>
       <c r="B23" s="6">
-        <f>G9*$K$2</f>
+        <f t="shared" si="1"/>
         <v>3441.0243600000003</v>
       </c>
-      <c r="D23" s="4">
+      <c r="F23" s="4">
         <v>8</v>
       </c>
-      <c r="E23" s="6">
+      <c r="G23" s="6">
         <f>G9*$K$3</f>
         <v>5161.536540000001</v>
       </c>
-      <c r="G23" s="4">
+      <c r="K23" s="4">
         <v>8</v>
       </c>
-      <c r="H23" s="6">
+      <c r="L23" s="6">
         <f>G9*$K$4</f>
         <v>860.25609000000009</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="P23" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="K23" s="4" t="s">
+      <c r="Q23" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L23" s="4" t="s">
+      <c r="R23" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>9</v>
       </c>
       <c r="B24" s="6">
-        <f>G10*$K$2</f>
+        <f t="shared" si="1"/>
         <v>3208.6152800000004</v>
       </c>
-      <c r="D24" s="4">
+      <c r="F24" s="4">
         <v>9</v>
       </c>
-      <c r="E24" s="6">
+      <c r="G24" s="6">
         <f>G10*$K$3</f>
         <v>4812.9229200000009</v>
       </c>
-      <c r="G24" s="4">
+      <c r="K24" s="4">
         <v>9</v>
       </c>
-      <c r="H24" s="6">
+      <c r="L24" s="6">
         <f>G10*$K$4</f>
         <v>802.15382000000011</v>
       </c>
-      <c r="J24" s="4">
+      <c r="P24" s="4">
         <v>3</v>
       </c>
-      <c r="K24" s="4">
+      <c r="Q24" s="4">
         <v>5750</v>
       </c>
-      <c r="L24" s="4">
+      <c r="R24" s="4">
         <v>500</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>10</v>
       </c>
       <c r="B25" s="6">
-        <f>G11*$K$2</f>
+        <f t="shared" si="1"/>
         <v>2633.49</v>
       </c>
-      <c r="D25" s="4">
+      <c r="F25" s="4">
         <v>10</v>
       </c>
-      <c r="E25" s="6">
+      <c r="G25" s="6">
         <f>G11*$K$3</f>
         <v>3950.2349999999997</v>
       </c>
-      <c r="G25" s="4">
+      <c r="K25" s="4">
         <v>10</v>
       </c>
-      <c r="H25" s="6">
+      <c r="L25" s="6">
         <f>G11*$K$4</f>
         <v>658.37249999999995</v>
       </c>
-      <c r="J25" s="4">
+      <c r="P25" s="4">
         <v>3</v>
       </c>
-      <c r="K25" s="4">
+      <c r="Q25" s="4">
         <v>3532</v>
       </c>
-      <c r="L25" s="4">
+      <c r="R25" s="4">
         <v>750</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="11">
+      <c r="B26" s="10">
         <f>SUM(B16:B25)</f>
         <v>28204.315728000001</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="F26" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E26" s="11">
-        <f>SUM(E16:E25)</f>
+      <c r="G26" s="10">
+        <f>SUM(G16:G25)</f>
         <v>42306.473591999995</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="K26" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H26" s="11">
-        <f>SUM(H16:H25)</f>
+      <c r="L26" s="10">
+        <f>SUM(L16:L25)</f>
         <v>7051.0789320000003</v>
       </c>
-      <c r="J26" s="4" t="s">
+      <c r="P26" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="K26" s="4">
-        <f>SUM(K24:K25)</f>
+      <c r="Q26" s="4">
+        <f>SUM(Q24:Q25)</f>
         <v>9282</v>
       </c>
-      <c r="L26" s="12"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="L27" s="12"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" s="11">
+        <f>C16+H16+M16</f>
+        <v>2969023.1999999997</v>
+      </c>
+      <c r="C31" s="11">
+        <f>B31/G2</f>
+        <v>3250</v>
+      </c>
+      <c r="D31" s="11">
+        <f>(F2/G2)-C31</f>
+        <v>-2155.3638920706308</v>
+      </c>
+      <c r="F31" s="11">
+        <f>(D31+D34)/2</f>
+        <v>-2517.1888277061762</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32" s="11">
+        <f>C17+H17+M17</f>
+        <v>2249314.6260000002</v>
+      </c>
+      <c r="C32" s="11">
+        <f>B32/G3</f>
+        <v>3249.9999999999995</v>
+      </c>
+      <c r="D32" s="11">
+        <f t="shared" ref="D32:D34" si="2">(F3/G3)-C32</f>
+        <v>362.21142924271362</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33" s="11">
+        <f>C18+H18+M18</f>
+        <v>4418110.4220000012</v>
+      </c>
+      <c r="C33" s="11">
+        <f t="shared" ref="C32:C34" si="3">B33/G4</f>
+        <v>3259.5268749581246</v>
+      </c>
+      <c r="D33" s="11">
+        <f t="shared" si="2"/>
+        <v>-1945.3009713165029</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>4</v>
+      </c>
+      <c r="B34" s="11">
+        <f>C19+H19+M19</f>
+        <v>6351180.0922000017</v>
+      </c>
+      <c r="C34" s="11">
+        <f t="shared" si="3"/>
+        <v>3865.9316487312535</v>
+      </c>
+      <c r="D34" s="11">
+        <f t="shared" si="2"/>
+        <v>-2879.0137633417216</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>